<commit_message>
tohle funguje a ulozi do excel
</commit_message>
<xml_diff>
--- a/ikea_products.xlsx
+++ b/ikea_products.xlsx
@@ -426,6 +426,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -445,12 +452,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Czech Price</t>
+          <t>Czech Price (CZK)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Poland Price</t>
+          <t>Poland Price (CZK)</t>
         </is>
       </c>
     </row>
@@ -551,13 +558,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="78" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -673,16 +688,6 @@
         <is>
           <t>250x60x236 cm</t>
         </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5">
-        <f>SUM(B2:B4)</f>
-        <v/>
-      </c>
-      <c r="C5">
-        <f>SUM(C2:C4)</f>
-        <v/>
       </c>
     </row>
   </sheetData>
@@ -696,13 +701,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="73" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -818,16 +831,6 @@
         <is>
           <t>250x60x236 cm</t>
         </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5">
-        <f>SUM(B2:B4)</f>
-        <v/>
-      </c>
-      <c r="C5">
-        <f>SUM(C2:C4)</f>
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vse funguje, ale neni to dokonale :D
</commit_message>
<xml_diff>
--- a/ikea_products.xlsx
+++ b/ikea_products.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,7 +427,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
@@ -464,86 +464,136 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PLATSA</t>
+          <t>FANBYN / Not available</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>394.374.11</t>
+          <t>492.284.74</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>280x57x261 cm</t>
+          <t>Not available</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>30160</v>
-      </c>
-      <c r="E2" t="n">
-        <v>24856.51878970604</v>
+        <v>1990</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PLATSA</t>
+          <t>VIDGA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>395.006.24</t>
+          <t>294.282.52</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>240x57x221 cm</t>
+          <t>Not available</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>20710</v>
+        <v>1246</v>
       </c>
       <c r="E3" t="n">
-        <v>17919.81587164854</v>
+        <v>1030.452245073759</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PAX / GRIMO/VIKEDAL</t>
+          <t>PAX / GRIMO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>694.780.23</t>
+          <t>994.329.72</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>250x60x236 cm</t>
+          <t>200x66x236 cm</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>22180</v>
+        <v>16010</v>
       </c>
       <c r="E4" t="n">
-        <v>16160.507160547</v>
+        <v>11234.44276946269</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PAX / TYSSEDAL</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>594.802.72</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>150x60x236 cm</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>15180</v>
+      </c>
+      <c r="E5" t="n">
+        <v>11812.50134596748</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NORRFLY / Not available</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>203.322.54</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>67 cm</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>399</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Total:</t>
         </is>
       </c>
-      <c r="B5" s="1" t="n"/>
-      <c r="C5" s="1" t="n"/>
-      <c r="D5" s="1">
-        <f>SUM(D2:D4)</f>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1">
+        <f>SUM(D2:D6)</f>
         <v/>
       </c>
-      <c r="E5" s="1">
-        <f>SUM(E2:E4)</f>
+      <c r="E7" s="1">
+        <f>SUM(E2:E6)</f>
         <v/>
       </c>
     </row>
@@ -558,7 +608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,11 +616,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="78" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -609,84 +659,140 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PLATSA</t>
+          <t>FANBYN</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6000.083972409066</v>
+        <v>395.8941347842852</v>
       </c>
       <c r="C2" t="n">
-        <v>30160</v>
+        <v>1990</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>394.374.11</t>
+          <t>492.284.74</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Šatní skříň s 11 dveřmi a 9 zás., bílá/FONNES, bílé,</t>
+          <t>Židle, bílá/vn./venkovní</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>280x57x261 cm</t>
+          <t>Not available</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PLATSA</t>
+          <t>VIDGA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4120.084186624395</v>
+        <v>247.8814532367936</v>
       </c>
       <c r="C3" t="n">
-        <v>20710</v>
+        <v>1246</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>395.006.24</t>
+          <t>294.282.52</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Šatní skříň s 9 dveřmi a 3 zásuv., bílá Kalbåden/vzor borovice FONNES, bílé,</t>
+          <t>Sada pro panelové závěsy, nástěnné upevnění/bílá</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>240x57x221 cm</t>
+          <t>Not available</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PAX / GRIMO/VIKEDAL</t>
+          <t>PAX / GRIMO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4412.528597746455</v>
+        <v>3185.057838138897</v>
       </c>
       <c r="C4" t="n">
-        <v>22180</v>
+        <v>16010</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>694.780.23</t>
+          <t>994.329.72</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Šatní skříň, bílá/šedá zrcadlové sklo,</t>
+          <t>Šatní sestava, bílá/bílá,</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>250x60x236 cm</t>
+          <t>200x66x236 cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PAX / TYSSEDAL</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3019.936163831884</v>
+      </c>
+      <c r="C5" t="n">
+        <v>15180</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>594.802.72</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Šatní sestava, bílá/zrcadlové sklo,</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>150x60x236 cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NORRFLY</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>79.37776873313055</v>
+      </c>
+      <c r="C6" t="n">
+        <v>399</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>203.322.54</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LED pásek, barva hliníku,</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>67 cm</t>
         </is>
       </c>
     </row>
@@ -701,7 +807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -709,11 +815,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="73" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="44" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -752,84 +858,148 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PLATSA</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>4945</v>
-      </c>
-      <c r="C2" t="n">
-        <v>24856.51878970604</v>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>394.374.11</t>
+          <t>Not available</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Szafa 11 drzwiami+9 szuflad, biały/FONNES biały,</t>
+          <t>Not available</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>280x57x261 cm</t>
+          <t>Not available</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PLATSA</t>
+          <t>VIDGA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3565</v>
+        <v>205</v>
       </c>
       <c r="C3" t="n">
-        <v>17919.81587164854</v>
+        <v>1030.452245073759</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>395.006.24</t>
+          <t>294.282.52</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Szafa 9 drzwi+3 szuflady, biały Kalbåden/żywy efekt sosny FONNES biały,</t>
+          <t>Zestaw do zasłon panelowych, ścienna/biały</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>240x57x221 cm</t>
+          <t>Not available</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PAX / GRIMO/VIKEDAL</t>
+          <t>PAX / GRIMO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3215</v>
+        <v>2235</v>
       </c>
       <c r="C4" t="n">
-        <v>16160.507160547</v>
+        <v>11234.44276946269</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>694.780.23</t>
+          <t>994.329.72</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Szafa, biały/szary lustro,</t>
+          <t>Kombinacja szafy, biały/biały,</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>250x60x236 cm</t>
+          <t>200x66x236 cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PAX / TYSSEDAL</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2350</v>
+      </c>
+      <c r="C5" t="n">
+        <v>11812.50134596748</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>594.802.72</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Kombinacja szafy, biały/lustro,</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>150x60x236 cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Not available</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update timesleep to not take too long
</commit_message>
<xml_diff>
--- a/ikea_products.xlsx
+++ b/ikea_products.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,7 +427,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
@@ -464,136 +464,86 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FANBYN / Not available</t>
+          <t>DRÖNA / KAVALKAD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>492.284.74</t>
+          <t>402.493.53</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>33x38x33 cm</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1990</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Not available</t>
-        </is>
+        <v>129</v>
+      </c>
+      <c r="E2" t="n">
+        <v>95.50533003122644</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>VIDGA</t>
+          <t>VARDAGEN / SANDVIVA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>294.282.52</t>
+          <t>002.947.24</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>23 cm</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1246</v>
+        <v>449</v>
       </c>
       <c r="E3" t="n">
-        <v>1030.452245073759</v>
+        <v>95.50533003122644</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PAX / GRIMO</t>
+          <t>SITTBRUNN / MÅLA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>994.329.72</t>
+          <t>805.394.83</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>200x66x236 cm</t>
+          <t>1 m</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>16010</v>
+        <v>49</v>
       </c>
       <c r="E4" t="n">
-        <v>11234.44276946269</v>
+        <v>25.13298158716485</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>PAX / TYSSEDAL</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>594.802.72</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>150x60x236 cm</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>15180</v>
-      </c>
-      <c r="E5" t="n">
-        <v>11812.50134596748</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>NORRFLY / Not available</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>203.322.54</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>67 cm</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>399</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Not available</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>Total:</t>
         </is>
       </c>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
-      <c r="D7" s="1">
-        <f>SUM(D2:D6)</f>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1">
+        <f>SUM(D2:D4)</f>
         <v/>
       </c>
-      <c r="E7" s="1">
-        <f>SUM(E2:E6)</f>
+      <c r="E5" s="1">
+        <f>SUM(E2:E4)</f>
         <v/>
       </c>
     </row>
@@ -608,7 +558,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,11 +566,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="50" customWidth="1" min="5" max="5"/>
+    <col width="31" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -659,140 +609,84 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FANBYN</t>
+          <t>DRÖNA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>395.8941347842852</v>
+        <v>25.66348913928281</v>
       </c>
       <c r="C2" t="n">
-        <v>1990</v>
+        <v>129</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>492.284.74</t>
+          <t>402.493.53</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Židle, bílá/vn./venkovní</t>
+          <t>Krabice, červená,</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>33x38x33 cm</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>VIDGA</t>
+          <t>VARDAGEN</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>247.8814532367936</v>
+        <v>89.32485754680606</v>
       </c>
       <c r="C3" t="n">
-        <v>1246</v>
+        <v>449</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>294.282.52</t>
+          <t>002.947.24</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sada pro panelové závěsy, nástěnné upevnění/bílá</t>
+          <t>Nůž na chléb, tmavě šedá,</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>23 cm</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PAX / GRIMO</t>
+          <t>SITTBRUNN</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3185.057838138897</v>
+        <v>9.748147037401997</v>
       </c>
       <c r="C4" t="n">
-        <v>16010</v>
+        <v>49</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>994.329.72</t>
+          <t>805.394.83</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Šatní sestava, bílá/bílá,</t>
+          <t>USB-A na USB-C, světle žlutá,</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>200x66x236 cm</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>PAX / TYSSEDAL</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3019.936163831884</v>
-      </c>
-      <c r="C5" t="n">
-        <v>15180</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>594.802.72</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Šatní sestava, bílá/zrcadlové sklo,</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>150x60x236 cm</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>NORRFLY</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>79.37776873313055</v>
-      </c>
-      <c r="C6" t="n">
-        <v>399</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>203.322.54</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>LED pásek, barva hliníku,</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>67 cm</t>
+          <t>1 m</t>
         </is>
       </c>
     </row>
@@ -807,7 +701,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -815,11 +709,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="44" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="29" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -858,55 +752,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Not available</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Not available</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Not available</t>
-        </is>
+          <t>KAVALKAD</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>19</v>
+      </c>
+      <c r="C2" t="n">
+        <v>95.50533003122644</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>002.677.06</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>Patelnia, czarny,</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>24 cm</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>VIDGA</t>
+          <t>SANDVIVA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>205</v>
+        <v>19</v>
       </c>
       <c r="C3" t="n">
-        <v>1030.452245073759</v>
+        <v>95.50533003122644</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>294.282.52</t>
+          <t>104.643.82</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Zestaw do zasłon panelowych, ścienna/biały</t>
+          <t>Rękawica, silikon/niebieski</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -918,86 +808,26 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PAX / GRIMO</t>
+          <t>MÅLA</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2235</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>11234.44276946269</v>
+        <v>25.13298158716485</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>994.329.72</t>
+          <t>904.565.90</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Kombinacja szafy, biały/biały,</t>
+          <t>Nożyczki</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
-        <is>
-          <t>200x66x236 cm</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>PAX / TYSSEDAL</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>2350</v>
-      </c>
-      <c r="C5" t="n">
-        <v>11812.50134596748</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>594.802.72</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Kombinacja szafy, biały/lustro,</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>150x60x236 cm</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Not available</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Not available</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Not available</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Not available</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Not available</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
         <is>
           <t>Not available</t>
         </is>

</xml_diff>